<commit_message>
Medal schedule by category: sort by display name
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/medalSchedule/ByCategory_A4.xlsx
+++ b/owlcms/src/main/resources/templates/medalSchedule/ByCategory_A4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgonzalez/Projects/Misc/owlcms4/owlcms/src/main/resources/templates/medalSchedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{504E7133-AE9F-C74F-B356-7BB4F903655E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E0617F-D3DF-C549-BABD-3E0D4E815888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="7860" windowWidth="39500" windowHeight="25100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="500" windowWidth="39500" windowHeight="23500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start List" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,18 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">jx:each(
+            <family val="34"/>
+          </rPr>
+          <t>jx:each(</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -126,27 +135,18 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">  items="</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>medalStatsPerCategory</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">"
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">  items="medalStatsPerCategory"</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -154,9 +154,18 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">  var="categoryStats"
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">  var="categoryStats"</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -164,9 +173,18 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">  lastCell="D6"
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">  orderBy="categoryStats.category.displayName"</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -174,7 +192,26 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">  lastCell="D6"</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
           </rPr>
           <t>)</t>
         </r>
@@ -261,10 +298,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Tahoma"/>
+      <family val="34"/>
     </font>
   </fonts>
   <fills count="3">
@@ -793,9 +830,7 @@
   </sheetPr>
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="179" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="179" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>